<commit_message>
minor changes to seedling plot analysis code
</commit_message>
<xml_diff>
--- a/Figures and Graphs/figures/seedling plot AICc table revised Aug2017.xlsx
+++ b/Figures and Graphs/figures/seedling plot AICc table revised Aug2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t xml:space="preserve">             K   AICc Delta_AICc AICcWt Cum.Wt      LL</t>
   </si>
@@ -96,13 +96,40 @@
   </si>
   <si>
     <t>Treatment</t>
+  </si>
+  <si>
+    <t>Carica papaya</t>
+  </si>
+  <si>
+    <t>Morinda citrifolia</t>
+  </si>
+  <si>
+    <t>Premna serratifolia</t>
+  </si>
+  <si>
+    <t>Psychotria mariana</t>
+  </si>
+  <si>
+    <t>Aglaia mariannensis</t>
+  </si>
+  <si>
+    <t>Ochrosia oppositifolia</t>
+  </si>
+  <si>
+    <t>With treatment</t>
+  </si>
+  <si>
+    <t>No treatment</t>
+  </si>
+  <si>
+    <t>AICc weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +166,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -181,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -214,6 +248,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,17 +588,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -686,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -703,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -720,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -737,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -754,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
@@ -771,7 +834,230 @@
         <v>1</v>
       </c>
     </row>
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="15">
+        <v>121.13</v>
+      </c>
+      <c r="D25" s="15">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="15">
+        <v>155.81</v>
+      </c>
+      <c r="D26" s="15">
+        <v>34.68</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="16">
+        <v>106.27</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="16">
+        <v>114.55</v>
+      </c>
+      <c r="D28" s="16">
+        <v>8.27</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="15">
+        <v>86.4</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="15">
+        <v>94.17</v>
+      </c>
+      <c r="D30" s="15">
+        <v>7.77</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="15">
+        <v>78.39</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="15">
+        <v>100.51</v>
+      </c>
+      <c r="D32" s="15">
+        <v>22.12</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="17">
+        <v>79.88</v>
+      </c>
+      <c r="D33" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="E33" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="17">
+        <v>79.36</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="17">
+        <v>48.94</v>
+      </c>
+      <c r="D35" s="17">
+        <v>2.72</v>
+      </c>
+      <c r="E35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="18">
+        <v>46.22</v>
+      </c>
+      <c r="D36" s="18">
+        <v>0</v>
+      </c>
+      <c r="E36" s="21">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>